<commit_message>
XG boost regression added
</commit_message>
<xml_diff>
--- a/venvs/my_excel_file.xlsx
+++ b/venvs/my_excel_file.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="input and output" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="output" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Accuracy Matrix" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -481,7 +482,7 @@
         <v>0.2</v>
       </c>
       <c r="H2" t="n">
-        <v>1444.069097488955</v>
+        <v>1704.686111630014</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +508,7 @@
         <v>0.4</v>
       </c>
       <c r="H3" t="n">
-        <v>1443.793894738421</v>
+        <v>1582.91248274873</v>
       </c>
     </row>
     <row r="4">
@@ -533,7 +534,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>1445.632712485068</v>
+        <v>1609.240885460225</v>
       </c>
     </row>
     <row r="5">
@@ -559,7 +560,7 @@
         <v>0.2</v>
       </c>
       <c r="H5" t="n">
-        <v>943.1548995440656</v>
+        <v>854.7006708577862</v>
       </c>
     </row>
     <row r="6">
@@ -585,7 +586,7 @@
         <v>0.4</v>
       </c>
       <c r="H6" t="n">
-        <v>932.9832244724906</v>
+        <v>762.4138356315652</v>
       </c>
     </row>
     <row r="7">
@@ -611,7 +612,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H7" t="n">
-        <v>948.7513976726733</v>
+        <v>834.6850544869509</v>
       </c>
     </row>
     <row r="8">
@@ -637,7 +638,7 @@
         <v>0.2</v>
       </c>
       <c r="H8" t="n">
-        <v>520.6920723443593</v>
+        <v>316.8816517039978</v>
       </c>
     </row>
     <row r="9">
@@ -663,7 +664,7 @@
         <v>0.4</v>
       </c>
       <c r="H9" t="n">
-        <v>502.5368749059851</v>
+        <v>227.4774295039226</v>
       </c>
     </row>
     <row r="10">
@@ -689,7 +690,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>530.4373335455826</v>
+        <v>310.5654023661726</v>
       </c>
     </row>
     <row r="11">
@@ -715,7 +716,7 @@
         <v>0.2</v>
       </c>
       <c r="H11" t="n">
-        <v>1430.386180144484</v>
+        <v>1676.763758119758</v>
       </c>
     </row>
     <row r="12">
@@ -741,7 +742,7 @@
         <v>0.4</v>
       </c>
       <c r="H12" t="n">
-        <v>1437.650226812111</v>
+        <v>1450.069178208779</v>
       </c>
     </row>
     <row r="13">
@@ -767,7 +768,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>1447.29318120043</v>
+        <v>1409.545851717702</v>
       </c>
     </row>
     <row r="14">
@@ -793,7 +794,7 @@
         <v>0.2</v>
       </c>
       <c r="H14" t="n">
-        <v>913.1102826072358</v>
+        <v>910.018337845763</v>
       </c>
     </row>
     <row r="15">
@@ -819,7 +820,7 @@
         <v>0.4</v>
       </c>
       <c r="H15" t="n">
-        <v>911.2573424029417</v>
+        <v>730.3549125210479</v>
       </c>
     </row>
     <row r="16">
@@ -845,7 +846,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>936.3176936157671</v>
+        <v>747.5298657828599</v>
       </c>
     </row>
     <row r="17">
@@ -871,7 +872,7 @@
         <v>0.2</v>
       </c>
       <c r="H17" t="n">
-        <v>476.9368048312467</v>
+        <v>436.7629706755599</v>
       </c>
     </row>
     <row r="18">
@@ -897,7 +898,7 @@
         <v>0.4</v>
       </c>
       <c r="H18" t="n">
-        <v>467.5232325899233</v>
+        <v>280.6690449284638</v>
       </c>
     </row>
     <row r="19">
@@ -923,7 +924,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H19" t="n">
-        <v>505.7406539777112</v>
+        <v>322.7999144929083</v>
       </c>
     </row>
     <row r="20">
@@ -949,7 +950,7 @@
         <v>0.2</v>
       </c>
       <c r="H20" t="n">
-        <v>1416.28227758509</v>
+        <v>1453.368635768806</v>
       </c>
     </row>
     <row r="21">
@@ -975,7 +976,7 @@
         <v>0.4</v>
       </c>
       <c r="H21" t="n">
-        <v>1430.465585127453</v>
+        <v>1153.961378675433</v>
       </c>
     </row>
     <row r="22">
@@ -1001,7 +1002,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>1447.438569984805</v>
+        <v>1088.407651713694</v>
       </c>
     </row>
     <row r="23">
@@ -1027,7 +1028,7 @@
         <v>0.2</v>
       </c>
       <c r="H23" t="n">
-        <v>907.1489411101022</v>
+        <v>822.5384554344778</v>
       </c>
     </row>
     <row r="24">
@@ -1053,7 +1054,7 @@
         <v>0.4</v>
       </c>
       <c r="H24" t="n">
-        <v>913.4244966945754</v>
+        <v>585.5954530518319</v>
       </c>
     </row>
     <row r="25">
@@ -1079,7 +1080,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H25" t="n">
-        <v>946.5707001198994</v>
+        <v>586.0958226153587</v>
       </c>
     </row>
     <row r="26">
@@ -1105,7 +1106,7 @@
         <v>0.2</v>
       </c>
       <c r="H26" t="n">
-        <v>478.1649949137266</v>
+        <v>471.3864673632135</v>
       </c>
     </row>
     <row r="27">
@@ -1131,7 +1132,7 @@
         <v>0.4</v>
       </c>
       <c r="H27" t="n">
-        <v>477.6720377583081</v>
+        <v>276.6715258979436</v>
       </c>
     </row>
     <row r="28">
@@ -1157,7 +1158,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H28" t="n">
-        <v>524.3767041641752</v>
+        <v>312.5586662609205</v>
       </c>
     </row>
     <row r="29">
@@ -1183,7 +1184,7 @@
         <v>0.2</v>
       </c>
       <c r="H29" t="n">
-        <v>1152.131807477278</v>
+        <v>960.618232136403</v>
       </c>
     </row>
     <row r="30">
@@ -1209,7 +1210,7 @@
         <v>0.4</v>
       </c>
       <c r="H30" t="n">
-        <v>1140.800986212277</v>
+        <v>1006.284923639372</v>
       </c>
     </row>
     <row r="31">
@@ -1235,7 +1236,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H31" t="n">
-        <v>1146.342226107212</v>
+        <v>1185.850922429772</v>
       </c>
     </row>
     <row r="32">
@@ -1261,7 +1262,7 @@
         <v>0.2</v>
       </c>
       <c r="H32" t="n">
-        <v>734.7696965203066</v>
+        <v>423.4251484224735</v>
       </c>
     </row>
     <row r="33">
@@ -1287,7 +1288,7 @@
         <v>0.4</v>
       </c>
       <c r="H33" t="n">
-        <v>715.014147236086</v>
+        <v>462.0208635971061</v>
       </c>
     </row>
     <row r="34">
@@ -1313,7 +1314,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H34" t="n">
-        <v>731.8976292756431</v>
+        <v>637.6093542260605</v>
       </c>
     </row>
     <row r="35">
@@ -1339,7 +1340,7 @@
         <v>0.2</v>
       </c>
       <c r="H35" t="n">
-        <v>406.4586350016853</v>
+        <v>178.3335811007846</v>
       </c>
     </row>
     <row r="36">
@@ -1365,7 +1366,7 @@
         <v>0.4</v>
       </c>
       <c r="H36" t="n">
-        <v>380.6653524496305</v>
+        <v>177.0415060578507</v>
       </c>
     </row>
     <row r="37">
@@ -1391,7 +1392,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>407.0256710401895</v>
+        <v>310.5662313084562</v>
       </c>
     </row>
     <row r="38">
@@ -1417,7 +1418,7 @@
         <v>0.2</v>
       </c>
       <c r="H38" t="n">
-        <v>1136.515507972707</v>
+        <v>941.230751522451</v>
       </c>
     </row>
     <row r="39">
@@ -1443,7 +1444,7 @@
         <v>0.4</v>
       </c>
       <c r="H39" t="n">
-        <v>1132.265800253959</v>
+        <v>899.6147662325794</v>
       </c>
     </row>
     <row r="40">
@@ -1469,7 +1470,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H40" t="n">
-        <v>1145.272118557971</v>
+        <v>1026.0935336984</v>
       </c>
     </row>
     <row r="41">
@@ -1495,7 +1496,7 @@
         <v>0.2</v>
       </c>
       <c r="H41" t="n">
-        <v>703.6941578017172</v>
+        <v>457.5382490612835</v>
       </c>
     </row>
     <row r="42">
@@ -1521,7 +1522,7 @@
         <v>0.4</v>
       </c>
       <c r="H42" t="n">
-        <v>691.8074403929209</v>
+        <v>424.9948570152389</v>
       </c>
     </row>
     <row r="43">
@@ -1547,7 +1548,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H43" t="n">
-        <v>717.607424752654</v>
+        <v>559.3033112319085</v>
       </c>
     </row>
     <row r="44">
@@ -1573,7 +1574,7 @@
         <v>0.2</v>
       </c>
       <c r="H44" t="n">
-        <v>362.6146515966973</v>
+        <v>247.4378421308387</v>
       </c>
     </row>
     <row r="45">
@@ -1599,7 +1600,7 @@
         <v>0.4</v>
       </c>
       <c r="H45" t="n">
-        <v>345.1441171335605</v>
+        <v>193.4959608855504</v>
       </c>
     </row>
     <row r="46">
@@ -1625,7 +1626,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>381.4287537334326</v>
+        <v>299.2919349249482</v>
       </c>
     </row>
     <row r="47">
@@ -1651,7 +1652,7 @@
         <v>0.2</v>
       </c>
       <c r="H47" t="n">
-        <v>1134.56572530079</v>
+        <v>806.8386776535771</v>
       </c>
     </row>
     <row r="48">
@@ -1677,7 +1678,7 @@
         <v>0.4</v>
       </c>
       <c r="H48" t="n">
-        <v>1137.307289802498</v>
+        <v>701.2125952441571</v>
       </c>
     </row>
     <row r="49">
@@ -1703,7 +1704,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H49" t="n">
-        <v>1157.122352224438</v>
+        <v>806.1933909446375</v>
       </c>
     </row>
     <row r="50">
@@ -1729,7 +1730,7 @@
         <v>0.2</v>
       </c>
       <c r="H50" t="n">
-        <v>706.7360466890142</v>
+        <v>415.4068604008259</v>
       </c>
     </row>
     <row r="51">
@@ -1755,7 +1756,7 @@
         <v>0.4</v>
       </c>
       <c r="H51" t="n">
-        <v>702.9870836455368</v>
+        <v>334.7226112754394</v>
       </c>
     </row>
     <row r="52">
@@ -1781,7 +1782,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H52" t="n">
-        <v>736.441006808159</v>
+        <v>458.3635493080553</v>
       </c>
     </row>
     <row r="53">
@@ -1807,7 +1808,7 @@
         <v>0.2</v>
       </c>
       <c r="H53" t="n">
-        <v>369.2258041224911</v>
+        <v>282.733872166943</v>
       </c>
     </row>
     <row r="54">
@@ -1833,7 +1834,7 @@
         <v>0.4</v>
       </c>
       <c r="H54" t="n">
-        <v>360.6224604669162</v>
+        <v>199.2870056873766</v>
       </c>
     </row>
     <row r="55">
@@ -1859,7 +1860,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H55" t="n">
-        <v>405.0747938341428</v>
+        <v>306.9584694147337</v>
       </c>
     </row>
     <row r="56">
@@ -1885,7 +1886,7 @@
         <v>0.2</v>
       </c>
       <c r="H56" t="n">
-        <v>867.4355502679346</v>
+        <v>540.292046288434</v>
       </c>
     </row>
     <row r="57">
@@ -1911,7 +1912,7 @@
         <v>0.4</v>
       </c>
       <c r="H57" t="n">
-        <v>845.8395352477207</v>
+        <v>718.2988742369675</v>
       </c>
     </row>
     <row r="58">
@@ -1937,7 +1938,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H58" t="n">
-        <v>855.5826084125952</v>
+        <v>1008.8281617147</v>
       </c>
     </row>
     <row r="59">
@@ -1963,7 +1964,7 @@
         <v>0.2</v>
       </c>
       <c r="H59" t="n">
-        <v>553.410392558312</v>
+        <v>290.1860083926538</v>
       </c>
     </row>
     <row r="60">
@@ -1989,7 +1990,7 @@
         <v>0.4</v>
       </c>
       <c r="H60" t="n">
-        <v>525.2438118663683</v>
+        <v>425.0861302554437</v>
       </c>
     </row>
     <row r="61">
@@ -2015,7 +2016,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H61" t="n">
-        <v>543.188043958485</v>
+        <v>664.5149333657328</v>
       </c>
     </row>
     <row r="62">
@@ -2041,7 +2042,7 @@
         <v>0.2</v>
       </c>
       <c r="H62" t="n">
-        <v>335.3030738426739</v>
+        <v>298.5694832968026</v>
       </c>
     </row>
     <row r="63">
@@ -2067,7 +2068,7 @@
         <v>0.4</v>
       </c>
       <c r="H63" t="n">
-        <v>303.3027658679753</v>
+        <v>354.4469353182872</v>
       </c>
     </row>
     <row r="64">
@@ -2093,7 +2094,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H64" t="n">
-        <v>327.5690061293453</v>
+        <v>504.9577419933012</v>
       </c>
     </row>
     <row r="65">
@@ -2119,7 +2120,7 @@
         <v>0.2</v>
       </c>
       <c r="H65" t="n">
-        <v>850.2140387349225</v>
+        <v>539.6083917580258</v>
       </c>
     </row>
     <row r="66">
@@ -2145,7 +2146,7 @@
         <v>0.4</v>
       </c>
       <c r="H66" t="n">
-        <v>834.8997516020437</v>
+        <v>650.9092792002606</v>
       </c>
     </row>
     <row r="67">
@@ -2171,7 +2172,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H67" t="n">
-        <v>851.4294922773706</v>
+        <v>903.0715059548023</v>
       </c>
     </row>
     <row r="68">
@@ -2197,7 +2198,7 @@
         <v>0.2</v>
       </c>
       <c r="H68" t="n">
-        <v>522.4177035242644</v>
+        <v>310.0579868136719</v>
       </c>
     </row>
     <row r="69">
@@ -2223,7 +2224,7 @@
         <v>0.4</v>
       </c>
       <c r="H69" t="n">
-        <v>501.2918803958078</v>
+        <v>392.2090444510407</v>
       </c>
     </row>
     <row r="70">
@@ -2249,7 +2250,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H70" t="n">
-        <v>527.3666596620259</v>
+        <v>604.5824196878602</v>
       </c>
     </row>
     <row r="71">
@@ -2275,7 +2276,7 @@
         <v>0.2</v>
       </c>
       <c r="H71" t="n">
-        <v>293.1587295911902</v>
+        <v>321.1198801129465</v>
       </c>
     </row>
     <row r="72">
@@ -2301,7 +2302,7 @@
         <v>0.4</v>
       </c>
       <c r="H72" t="n">
-        <v>268.6632589423591</v>
+        <v>339.7010123904282</v>
       </c>
     </row>
     <row r="73">
@@ -2327,7 +2328,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H73" t="n">
-        <v>302.0004228843031</v>
+        <v>475.5638143173289</v>
       </c>
     </row>
     <row r="74">
@@ -2353,7 +2354,7 @@
         <v>0.2</v>
       </c>
       <c r="H74" t="n">
-        <v>860.6186799256515</v>
+        <v>504.2619939820663</v>
       </c>
     </row>
     <row r="75">
@@ -2379,7 +2380,7 @@
         <v>0.4</v>
       </c>
       <c r="H75" t="n">
-        <v>852.0178955987816</v>
+        <v>563.7437843127781</v>
       </c>
     </row>
     <row r="76">
@@ -2405,7 +2406,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H76" t="n">
-        <v>874.4898408492513</v>
+        <v>799.1911489125321</v>
       </c>
     </row>
     <row r="77">
@@ -2431,7 +2432,7 @@
         <v>0.2</v>
       </c>
       <c r="H77" t="n">
-        <v>534.4755163622465</v>
+        <v>320.7566736636825</v>
       </c>
     </row>
     <row r="78">
@@ -2457,7 +2458,7 @@
         <v>0.4</v>
       </c>
       <c r="H78" t="n">
-        <v>521.0937472449255</v>
+        <v>366.6123722390209</v>
       </c>
     </row>
     <row r="79">
@@ -2483,7 +2484,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H79" t="n">
-        <v>554.0040114368959</v>
+        <v>574.9487739104005</v>
       </c>
     </row>
     <row r="80">
@@ -2509,7 +2510,7 @@
         <v>0.2</v>
       </c>
       <c r="H80" t="n">
-        <v>305.0388192104156</v>
+        <v>362.3888998161233</v>
       </c>
     </row>
     <row r="81">
@@ -2535,7 +2536,7 @@
         <v>0.4</v>
       </c>
       <c r="H81" t="n">
-        <v>288.9215482601203</v>
+        <v>362.3549929478096</v>
       </c>
     </row>
     <row r="82">
@@ -2561,7 +2562,7 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="H82" t="n">
-        <v>329.6958119487533</v>
+        <v>508.1251222500279</v>
       </c>
     </row>
   </sheetData>
@@ -2575,7 +2576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2587,653 +2588,572 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="BR1" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="BS1" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="BT1" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="BU1" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="BV1" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="BW1" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="BX1" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="BY1" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="BZ1" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="CA1" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="CB1" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="CC1" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="CD1" s="1" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1444.069097488955</v>
+        <v>1704.686111630014</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1582.91248274873</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1609.240885460225</v>
+      </c>
+      <c r="E2" t="n">
+        <v>854.7006708577862</v>
+      </c>
+      <c r="F2" t="n">
+        <v>762.4138356315652</v>
+      </c>
+      <c r="G2" t="n">
+        <v>834.6850544869509</v>
+      </c>
+      <c r="H2" t="n">
+        <v>316.8816517039978</v>
+      </c>
+      <c r="I2" t="n">
+        <v>227.4774295039226</v>
+      </c>
+      <c r="J2" t="n">
+        <v>310.5654023661726</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1676.763758119758</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1450.069178208779</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1409.545851717702</v>
+      </c>
+      <c r="N2" t="n">
+        <v>910.018337845763</v>
+      </c>
+      <c r="O2" t="n">
+        <v>730.3549125210479</v>
+      </c>
+      <c r="P2" t="n">
+        <v>747.5298657828599</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>436.7629706755599</v>
+      </c>
+      <c r="R2" t="n">
+        <v>280.6690449284638</v>
+      </c>
+      <c r="S2" t="n">
+        <v>322.7999144929083</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1453.368635768806</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1153.961378675433</v>
+      </c>
+      <c r="V2" t="n">
+        <v>1088.407651713694</v>
+      </c>
+      <c r="W2" t="n">
+        <v>822.5384554344778</v>
+      </c>
+      <c r="X2" t="n">
+        <v>585.5954530518319</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>586.0958226153587</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>471.3864673632135</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>276.6715258979436</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>312.5586662609205</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>960.618232136403</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1006.284923639372</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1185.850922429772</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>423.4251484224735</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>462.0208635971061</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>637.6093542260605</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>178.3335811007846</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>177.0415060578507</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>310.5662313084562</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>941.230751522451</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>899.6147662325794</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1026.0935336984</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>457.5382490612835</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>424.9948570152389</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>559.3033112319085</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>247.4378421308387</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>193.4959608855504</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>299.2919349249482</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>806.8386776535771</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>701.2125952441571</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>806.1933909446375</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>415.4068604008259</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>334.7226112754394</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>458.3635493080553</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>282.733872166943</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>199.2870056873766</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>306.9584694147337</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>540.292046288434</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>718.2988742369675</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>1008.8281617147</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>290.1860083926538</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>425.0861302554437</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>664.5149333657328</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>298.5694832968026</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>354.4469353182872</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>504.9577419933012</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>539.6083917580258</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>650.9092792002606</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>903.0715059548023</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>310.0579868136719</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>392.2090444510407</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>604.5824196878602</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>321.1198801129465</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>339.7010123904282</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>475.5638143173289</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>504.2619939820663</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>563.7437843127781</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>799.1911489125321</v>
+      </c>
+      <c r="BY2" t="n">
+        <v>320.7566736636825</v>
+      </c>
+      <c r="BZ2" t="n">
+        <v>366.6123722390209</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>574.9487739104005</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>362.3888998161233</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>362.3549929478096</v>
+      </c>
+      <c r="CD2" t="n">
+        <v>508.1251222500279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>mean squared error (MSE)</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.004332851662157621</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1443.793894738421</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>root Mean Square Error (RMSE)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06582440020355386</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>1445.632712485068</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mean absolute error</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.05435177022968006</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>943.1548995440656</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>932.9832244724906</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>948.7513976726733</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>520.6920723443593</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>502.5368749059851</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>530.4373335455826</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1430.386180144484</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1437.650226812111</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1447.29318120043</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>913.1102826072358</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>911.2573424029417</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>936.3176936157671</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>476.9368048312467</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>467.5232325899233</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>505.7406539777112</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1416.28227758509</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1430.465585127453</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1447.438569984805</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>907.1489411101022</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>913.4244966945754</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>946.5707001198994</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>478.1649949137266</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>477.6720377583081</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>524.3767041641752</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1152.131807477278</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>1140.800986212277</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>1146.342226107212</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>734.7696965203066</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>715.014147236086</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>731.8976292756431</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>406.4586350016853</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>380.6653524496305</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>407.0256710401895</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>1136.515507972707</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>1132.265800253959</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="n">
-        <v>1145.272118557971</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="n">
-        <v>703.6941578017172</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>691.8074403929209</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="n">
-        <v>717.607424752654</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="n">
-        <v>362.6146515966973</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>345.1441171335605</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="n">
-        <v>381.4287537334326</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="n">
-        <v>1134.56572530079</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="n">
-        <v>1137.307289802498</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="n">
-        <v>1157.122352224438</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="n">
-        <v>706.7360466890142</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="n">
-        <v>702.9870836455368</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="n">
-        <v>736.441006808159</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="n">
-        <v>369.2258041224911</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="n">
-        <v>360.6224604669162</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="n">
-        <v>405.0747938341428</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="n">
-        <v>867.4355502679346</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="n">
-        <v>845.8395352477207</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="n">
-        <v>855.5826084125952</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="n">
-        <v>553.410392558312</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>525.2438118663683</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>543.188043958485</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="n">
-        <v>335.3030738426739</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>303.3027658679753</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>327.5690061293453</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>850.2140387349225</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>834.8997516020437</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="n">
-        <v>851.4294922773706</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>522.4177035242644</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>501.2918803958078</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>527.3666596620259</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="n">
-        <v>293.1587295911902</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="n">
-        <v>268.6632589423591</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>302.0004228843031</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="n">
-        <v>860.6186799256515</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>852.0178955987816</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>874.4898408492513</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>534.4755163622465</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>521.0937472449255</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>554.0040114368959</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>305.0388192104156</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>288.9215482601203</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="n">
-        <v>329.6958119487533</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mean absolute percentage error</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4.829613697416906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>